<commit_message>
wilson amplitude visualizer and code
</commit_message>
<xml_diff>
--- a/Assignment3/inferences/dm_stats.xlsx
+++ b/Assignment3/inferences/dm_stats.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbhar\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fe52e46c4edfd6cc/Documents/ASU/Subjects/DM/Project/datamining/Assignment3/inferences/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="8" documentId="EED491B2FF52BBF8463439437EE262A93533EC49" xr6:coauthVersionLast="23" xr6:coauthVersionMax="23" xr10:uidLastSave="{B5FEC3A7-F851-47AD-B8D5-A74CCE4D30CC}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9636" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="16">
   <si>
     <t>Feature No.</t>
   </si>
@@ -57,12 +58,27 @@
   </si>
   <si>
     <t>Non Eating (Mean)</t>
+  </si>
+  <si>
+    <t>RMS</t>
+  </si>
+  <si>
+    <t>Entropy</t>
+  </si>
+  <si>
+    <t>Mean Absolute Value</t>
+  </si>
+  <si>
+    <t>Wilson Amplitude</t>
+  </si>
+  <si>
+    <t>Zero Crossing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -407,11 +423,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -421,9 +437,12 @@
     <col min="3" max="3" width="27.88671875" customWidth="1"/>
     <col min="4" max="4" width="21.109375" customWidth="1"/>
     <col min="5" max="5" width="24.109375" customWidth="1"/>
+    <col min="11" max="11" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -448,8 +467,23 @@
       <c r="H1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -469,7 +503,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -489,7 +523,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -509,7 +543,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -529,7 +563,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -549,7 +583,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -569,7 +603,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -589,7 +623,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -609,7 +643,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -629,7 +663,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -649,7 +683,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -672,7 +706,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -692,7 +726,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -712,7 +746,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -729,7 +763,7 @@
         <v>-0.77659999999999996</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>

</xml_diff>